<commit_message>
restructured for extensibility into sections beyond 'Eon View'
</commit_message>
<xml_diff>
--- a/GEO.xlsx
+++ b/GEO.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="190">
   <si>
     <t>Data for geo timeline:</t>
   </si>
@@ -1311,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2004,7 +2004,9 @@
       <c r="G52" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H52" s="18"/>
+      <c r="H52" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="I52" s="19"/>
       <c r="J52" s="20"/>
     </row>
@@ -2035,9 +2037,6 @@
       <c r="J55" s="20"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="H56" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="I56" s="10" t="s">
         <v>20</v>
       </c>
@@ -2236,6 +2235,9 @@
       </c>
     </row>
     <row r="92" spans="1:10" s="2" customFormat="1">
+      <c r="A92" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="F92" s="3"/>
       <c r="G92" s="4"/>
       <c r="H92" s="7"/>
@@ -2445,6 +2447,9 @@
       </c>
     </row>
     <row r="120" spans="1:10" s="2" customFormat="1">
+      <c r="A120" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="F120" s="3"/>
       <c r="G120" s="4"/>
       <c r="H120" s="7"/>

</xml_diff>

<commit_message>
updated most items to ICS chart
</commit_message>
<xml_diff>
--- a/GEO.xlsx
+++ b/GEO.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="190">
   <si>
     <t>Data for geo timeline:</t>
   </si>
@@ -487,9 +487,6 @@
     <t>Earliest Oxygen / Photosynthesis</t>
   </si>
   <si>
-    <t>542 M</t>
-  </si>
-  <si>
     <t>Earliest possible life (single-celled)</t>
   </si>
   <si>
@@ -614,6 +611,9 @@
   </si>
   <si>
     <t>New Mexico Bureau of Geology and Mineral Resources</t>
+  </si>
+  <si>
+    <t>540 M</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1312,7 @@
   <dimension ref="A1:J130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1409,10 +1409,10 @@
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1">
       <c r="A6" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E6" s="53"/>
       <c r="F6" s="52"/>
@@ -1426,7 +1426,7 @@
         <v>144</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E7" s="53"/>
       <c r="F7" s="42" t="s">
@@ -1442,7 +1442,7 @@
     <row r="8" spans="1:10" s="15" customFormat="1">
       <c r="A8" s="21"/>
       <c r="B8" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E8" s="53"/>
       <c r="F8" s="43"/>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="9" spans="1:10" s="15" customFormat="1">
       <c r="A9" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="2"/>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="10" spans="1:10" s="15" customFormat="1">
       <c r="A10" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10" s="21"/>
       <c r="E10" s="53"/>
@@ -1496,7 +1496,7 @@
         <v>145</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C12" s="15"/>
       <c r="E12" s="53"/>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C14" s="15"/>
       <c r="E14" s="53"/>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C16" s="15"/>
       <c r="E16" s="53"/>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E17" s="53"/>
       <c r="F17" s="43"/>
@@ -1578,7 +1578,7 @@
         <v>127</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C19" s="15"/>
       <c r="E19" s="53"/>
@@ -1597,7 +1597,7 @@
         <v>127</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C20" s="15"/>
       <c r="E20" s="53"/>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E23" s="53"/>
       <c r="F23" s="43"/>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1649,17 +1649,17 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E25" s="53"/>
       <c r="F25" s="43"/>
       <c r="H25" s="45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1670,12 +1670,12 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E27" s="53"/>
       <c r="F27" s="43"/>
       <c r="H27" s="45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1691,7 +1691,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1703,7 +1703,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E30" s="53"/>
       <c r="F30" s="43"/>
@@ -1711,7 +1711,7 @@
         <v>131</v>
       </c>
       <c r="H30" s="45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="15" customFormat="1">
@@ -1731,10 +1731,10 @@
     </row>
     <row r="32" spans="1:10" s="15" customFormat="1">
       <c r="A32" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" t="s">
         <v>157</v>
-      </c>
-      <c r="B32" t="s">
-        <v>158</v>
       </c>
       <c r="C32"/>
       <c r="E32" s="53"/>
@@ -1746,10 +1746,10 @@
     </row>
     <row r="33" spans="1:10" s="15" customFormat="1">
       <c r="A33" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="34" spans="1:10" s="15" customFormat="1">
       <c r="A34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B34"/>
       <c r="C34"/>
@@ -1770,7 +1770,7 @@
       <c r="F34" s="43"/>
       <c r="G34" s="36"/>
       <c r="H34" s="45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I34" s="19"/>
       <c r="J34" s="20"/>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1801,13 +1801,13 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E37" s="53"/>
       <c r="F37" s="43"/>
       <c r="G37" s="36"/>
       <c r="H37" s="45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1815,7 +1815,7 @@
         <v>14</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E38" s="53"/>
       <c r="F38" s="43"/>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1836,7 +1836,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E40" s="53"/>
       <c r="F40" s="43"/>
@@ -1861,7 +1861,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C42" s="15"/>
       <c r="E42" s="53"/>
@@ -1871,10 +1871,10 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B43" s="21" t="s">
         <v>154</v>
-      </c>
-      <c r="B43" s="21" t="s">
-        <v>155</v>
       </c>
       <c r="C43" s="15"/>
       <c r="E43" s="53"/>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="44" spans="1:10" s="15" customFormat="1">
       <c r="A44" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="45" spans="1:10" s="15" customFormat="1">
       <c r="A45" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E45" s="53"/>
       <c r="F45" s="43"/>
@@ -1911,10 +1911,10 @@
     </row>
     <row r="46" spans="1:10" s="15" customFormat="1">
       <c r="A46" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" s="21" t="s">
         <v>167</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>168</v>
       </c>
       <c r="E46" s="53"/>
       <c r="F46" s="43"/>
@@ -1925,7 +1925,7 @@
     </row>
     <row r="47" spans="1:10" s="15" customFormat="1">
       <c r="A47" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="48" spans="1:10" s="15" customFormat="1">
       <c r="A48" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="43"/>
@@ -1952,10 +1952,10 @@
     </row>
     <row r="49" spans="1:10" s="15" customFormat="1">
       <c r="A49" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E49" s="31"/>
       <c r="F49" s="43"/>
@@ -1967,7 +1967,7 @@
     <row r="50" spans="1:10" s="15" customFormat="1">
       <c r="A50" s="21"/>
       <c r="B50" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E50" s="31"/>
       <c r="F50" s="43"/>
@@ -1978,10 +1978,10 @@
     </row>
     <row r="51" spans="1:10" s="6" customFormat="1" ht="16" thickBot="1">
       <c r="A51" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E51" s="24"/>
       <c r="F51" s="49"/>
@@ -1992,10 +1992,10 @@
     </row>
     <row r="52" spans="1:10" s="15" customFormat="1" ht="16" thickTop="1">
       <c r="A52" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="1" t="s">
@@ -2046,9 +2046,14 @@
         <v>21</v>
       </c>
     </row>
+    <row r="58" spans="1:10">
+      <c r="A58" t="s">
+        <v>189</v>
+      </c>
+    </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="H59" s="8" t="s">
         <v>22</v>
@@ -2548,7 +2553,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2556,12 +2561,12 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="C3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>